<commit_message>
create func from insert block into zone
</commit_message>
<xml_diff>
--- a/cad/data.xlsx
+++ b/cad/data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutomaticCad\cad\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\4 PProject\AutovaticCad\cad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CF5223-DDE8-45E4-8648-3965F8483B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5910" yWindow="0" windowWidth="19230" windowHeight="15750" xr2:uid="{9A125CD0-8040-4073-88E8-ADA0FAC39D96}"/>
+    <workbookView xWindow="5910" yWindow="0" windowWidth="19230" windowHeight="15750"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="3" r:id="rId1"/>
@@ -25,7 +24,7 @@
     <definedName name="d_ovik">#REF!</definedName>
     <definedName name="n_visio">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="146">
   <si>
     <t>Наименование</t>
   </si>
@@ -220,9 +219,6 @@
     <t>Откуда</t>
   </si>
   <si>
-    <t>ТКШ</t>
-  </si>
-  <si>
     <t>ЭВ</t>
   </si>
   <si>
@@ -232,21 +228,6 @@
     <t>Тепло</t>
   </si>
   <si>
-    <t>История клуба</t>
-  </si>
-  <si>
-    <t>Фотозона</t>
-  </si>
-  <si>
-    <t>Удар нападающего</t>
-  </si>
-  <si>
-    <t>Триединство волеболиста</t>
-  </si>
-  <si>
-    <t>Управление</t>
-  </si>
-  <si>
     <t>Wize</t>
   </si>
   <si>
@@ -349,9 +330,6 @@
     <t>Высота</t>
   </si>
   <si>
-    <t>Матч с Про</t>
-  </si>
-  <si>
     <t>ЭВ-1</t>
   </si>
   <si>
@@ -388,9 +366,6 @@
     <t>ЭВ-6</t>
   </si>
   <si>
-    <t>История клуба. Проекция</t>
-  </si>
-  <si>
     <t>Потолок</t>
   </si>
   <si>
@@ -482,13 +457,28 @@
   </si>
   <si>
     <t>Вывод</t>
+  </si>
+  <si>
+    <t>Зона 1</t>
+  </si>
+  <si>
+    <t>Зона 2</t>
+  </si>
+  <si>
+    <t>Зона 3</t>
+  </si>
+  <si>
+    <t>Зона 4</t>
+  </si>
+  <si>
+    <t>Зона 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -606,7 +596,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Стиль 1" xfId="1" xr:uid="{EA3F791E-525E-434E-B27C-1BB669B3A9D9}"/>
+    <cellStyle name="Стиль 1" xfId="1"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -831,15 +821,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0715982B-A757-4117-A94A-25CAFA92E94F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="7" style="2" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" style="2" customWidth="1"/>
@@ -862,12 +852,12 @@
     <col min="19" max="16384" width="5.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>0</v>
@@ -891,7 +881,7 @@
         <v>56</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>57</v>
@@ -900,13 +890,13 @@
         <v>58</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="P1" s="6" t="s">
         <v>59</v>
@@ -915,7 +905,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -936,10 +926,10 @@
         <v>1</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>65</v>
+        <v>141</v>
       </c>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
@@ -953,14 +943,14 @@
         <v>300</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="Q2" s="6" t="str">
         <f t="shared" ref="Q2:Q39" si="1">IF(N2&lt;&gt;"",$N$41,"")</f>
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -972,7 +962,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>9</v>
@@ -981,10 +971,10 @@
         <v>1</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>65</v>
+        <v>142</v>
       </c>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
@@ -1001,7 +991,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1022,10 +1012,10 @@
         <v>1</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>65</v>
+        <v>143</v>
       </c>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
@@ -1042,7 +1032,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1063,13 +1053,13 @@
         <v>1</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>65</v>
+        <v>144</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="K5" s="6">
         <v>150</v>
@@ -1089,7 +1079,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -1112,13 +1102,13 @@
         <v>1</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>117</v>
+        <v>145</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="K6" s="6">
         <v>211</v>
@@ -1130,17 +1120,17 @@
       </c>
       <c r="N6" s="6"/>
       <c r="O6" s="6" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="Q6" s="6" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17">
       <c r="A7" s="6">
         <v>5</v>
       </c>
@@ -1163,13 +1153,13 @@
         <v>1</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="K7" s="6">
         <v>211</v>
@@ -1181,17 +1171,17 @@
       </c>
       <c r="N7" s="6"/>
       <c r="O7" s="6" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="Q7" s="6" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17">
       <c r="A8" s="6">
         <v>6</v>
       </c>
@@ -1202,10 +1192,10 @@
         <v>18</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>9</v>
@@ -1214,10 +1204,10 @@
         <v>1</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
@@ -1234,7 +1224,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17">
       <c r="A9" s="6">
         <v>6</v>
       </c>
@@ -1245,10 +1235,10 @@
         <v>18</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>9</v>
@@ -1257,10 +1247,10 @@
         <v>1</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>117</v>
+        <v>143</v>
       </c>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
@@ -1277,7 +1267,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17">
       <c r="A10" s="6">
         <v>12</v>
       </c>
@@ -1298,10 +1288,10 @@
         <v>1</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>66</v>
+        <v>144</v>
       </c>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
@@ -1315,14 +1305,14 @@
         <v>1500</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="Q10" s="6" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17">
       <c r="A11" s="6">
         <v>12.1</v>
       </c>
@@ -1341,10 +1331,10 @@
         <v>1</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>66</v>
+        <v>145</v>
       </c>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
@@ -1361,7 +1351,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17">
       <c r="A12" s="6">
         <v>13</v>
       </c>
@@ -1382,10 +1372,10 @@
         <v>1</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>66</v>
+        <v>141</v>
       </c>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
@@ -1402,7 +1392,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17">
       <c r="A13" s="6">
         <v>14</v>
       </c>
@@ -1423,13 +1413,13 @@
         <v>1</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>66</v>
+        <v>142</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="K13" s="6">
         <v>1200</v>
@@ -1449,7 +1439,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17">
       <c r="A14" s="6">
         <v>15</v>
       </c>
@@ -1470,10 +1460,10 @@
         <v>1</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>66</v>
+        <v>143</v>
       </c>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
@@ -1490,7 +1480,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17">
       <c r="A15" s="6">
         <v>17</v>
       </c>
@@ -1511,10 +1501,10 @@
         <v>1</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>67</v>
+        <v>144</v>
       </c>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
@@ -1528,14 +1518,14 @@
         <v>1500</v>
       </c>
       <c r="P15" s="6" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="Q15" s="6" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="13.5" customHeight="1">
       <c r="A16" s="6">
         <v>17.100000000000001</v>
       </c>
@@ -1544,10 +1534,10 @@
         <v>26</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F16" s="9" t="s">
         <v>9</v>
@@ -1556,10 +1546,10 @@
         <v>1</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>67</v>
+        <v>145</v>
       </c>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
@@ -1576,7 +1566,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17">
       <c r="A17" s="6">
         <v>18</v>
       </c>
@@ -1597,10 +1587,10 @@
         <v>1</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>67</v>
+        <v>141</v>
       </c>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
@@ -1617,7 +1607,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17">
       <c r="A18" s="6">
         <v>19</v>
       </c>
@@ -1638,13 +1628,13 @@
         <v>1</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>67</v>
+        <v>142</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="K18" s="6">
         <v>1200</v>
@@ -1664,7 +1654,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17">
       <c r="A19" s="6">
         <v>20</v>
       </c>
@@ -1686,7 +1676,7 @@
       </c>
       <c r="H19" s="6"/>
       <c r="I19" s="6" t="s">
-        <v>67</v>
+        <v>143</v>
       </c>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
@@ -1703,7 +1693,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17">
       <c r="A20" s="6">
         <v>21</v>
       </c>
@@ -1724,13 +1714,13 @@
         <v>1</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>104</v>
+        <v>144</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="K20" s="6">
         <v>550</v>
@@ -1742,17 +1732,17 @@
       </c>
       <c r="N20" s="6"/>
       <c r="O20" s="6" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="P20" s="6" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="Q20" s="6" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17">
       <c r="A21" s="6">
         <v>22</v>
       </c>
@@ -1769,9 +1759,11 @@
       <c r="F21" s="9"/>
       <c r="G21" s="8"/>
       <c r="H21" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="I21" s="6"/>
+        <v>132</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>145</v>
+      </c>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
@@ -1781,7 +1773,7 @@
       <c r="P21" s="6"/>
       <c r="Q21" s="6"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17">
       <c r="A22" s="6">
         <v>23</v>
       </c>
@@ -1790,10 +1782,10 @@
         <v>18</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F22" s="9" t="s">
         <v>9</v>
@@ -1802,10 +1794,10 @@
         <v>1</v>
       </c>
       <c r="H22" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="I22" s="6" t="s">
         <v>141</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>104</v>
       </c>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
@@ -1822,7 +1814,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17">
       <c r="A23" s="6">
         <v>29</v>
       </c>
@@ -1843,13 +1835,13 @@
         <v>1</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>104</v>
+        <v>142</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="K23" s="6">
         <v>50</v>
@@ -1864,14 +1856,14 @@
         <v>1000</v>
       </c>
       <c r="P23" s="6" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="Q23" s="6" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17">
       <c r="A24" s="6">
         <v>30</v>
       </c>
@@ -1894,13 +1886,13 @@
         <v>1</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="K24" s="6">
         <v>1000</v>
@@ -1912,17 +1904,17 @@
       </c>
       <c r="N24" s="6"/>
       <c r="O24" s="6" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="P24" s="6" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="Q24" s="6" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17">
       <c r="A25" s="6">
         <v>30</v>
       </c>
@@ -1945,13 +1937,13 @@
         <v>1</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>68</v>
+        <v>144</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="K25" s="6">
         <v>1000</v>
@@ -1963,17 +1955,17 @@
       </c>
       <c r="N25" s="6"/>
       <c r="O25" s="6" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="P25" s="6" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="Q25" s="6" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17">
       <c r="A26" s="6">
         <v>31</v>
       </c>
@@ -1996,9 +1988,11 @@
         <v>1</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="I26" s="6"/>
+        <v>111</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>145</v>
+      </c>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
@@ -2008,7 +2002,7 @@
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17">
       <c r="A27" s="6">
         <v>31</v>
       </c>
@@ -2031,9 +2025,11 @@
         <v>1</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="I27" s="6"/>
+        <v>136</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>141</v>
+      </c>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
@@ -2043,7 +2039,7 @@
       <c r="P27" s="6"/>
       <c r="Q27" s="6"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17">
       <c r="A28" s="6">
         <v>32</v>
       </c>
@@ -2054,10 +2050,10 @@
         <v>18</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F28" s="9" t="s">
         <v>9</v>
@@ -2066,10 +2062,10 @@
         <v>1</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>68</v>
+        <v>142</v>
       </c>
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
@@ -2086,7 +2082,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17">
       <c r="A29" s="6">
         <v>32</v>
       </c>
@@ -2097,10 +2093,10 @@
         <v>18</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F29" s="9" t="s">
         <v>9</v>
@@ -2109,10 +2105,10 @@
         <v>1</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
@@ -2129,7 +2125,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17">
       <c r="A30" s="6">
         <v>34</v>
       </c>
@@ -2150,10 +2146,10 @@
         <v>1</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>68</v>
+        <v>144</v>
       </c>
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
@@ -2164,14 +2160,14 @@
         <v>300</v>
       </c>
       <c r="P30" s="6" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="Q30" s="6" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17">
       <c r="A31" s="6">
         <v>39</v>
       </c>
@@ -2182,22 +2178,22 @@
         <v>39</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E31" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="8">
+        <v>1</v>
+      </c>
+      <c r="H31" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F31" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G31" s="8">
-        <v>1</v>
-      </c>
-      <c r="H31" s="6" t="s">
-        <v>80</v>
-      </c>
       <c r="I31" s="6" t="s">
-        <v>68</v>
+        <v>145</v>
       </c>
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
@@ -2209,14 +2205,14 @@
       <c r="N31" s="6"/>
       <c r="O31" s="6"/>
       <c r="P31" s="6" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="Q31" s="6" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17">
       <c r="A32" s="6">
         <v>39</v>
       </c>
@@ -2227,10 +2223,10 @@
         <v>39</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F32" s="9" t="s">
         <v>9</v>
@@ -2239,10 +2235,10 @@
         <v>1</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>68</v>
+        <v>141</v>
       </c>
       <c r="J32" s="6"/>
       <c r="K32" s="6"/>
@@ -2254,14 +2250,14 @@
       <c r="N32" s="6"/>
       <c r="O32" s="6"/>
       <c r="P32" s="6" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="Q32" s="6" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17">
       <c r="A33" s="6">
         <v>39</v>
       </c>
@@ -2272,10 +2268,10 @@
         <v>39</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F33" s="9" t="s">
         <v>9</v>
@@ -2284,10 +2280,10 @@
         <v>1</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>68</v>
+        <v>142</v>
       </c>
       <c r="J33" s="6"/>
       <c r="K33" s="6"/>
@@ -2299,14 +2295,14 @@
       <c r="N33" s="6"/>
       <c r="O33" s="6"/>
       <c r="P33" s="6" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="Q33" s="6" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17">
       <c r="A34" s="6">
         <v>39</v>
       </c>
@@ -2317,10 +2313,10 @@
         <v>39</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F34" s="9" t="s">
         <v>9</v>
@@ -2329,10 +2325,10 @@
         <v>1</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="J34" s="6"/>
       <c r="K34" s="6"/>
@@ -2344,14 +2340,14 @@
       <c r="N34" s="6"/>
       <c r="O34" s="6"/>
       <c r="P34" s="6" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="Q34" s="6" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17">
       <c r="A35" s="6">
         <v>48</v>
       </c>
@@ -2360,7 +2356,7 @@
         <v>40</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>41</v>
@@ -2372,10 +2368,10 @@
         <v>1</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>69</v>
+        <v>144</v>
       </c>
       <c r="J35" s="6"/>
       <c r="K35" s="6"/>
@@ -2389,14 +2385,14 @@
         <v>30</v>
       </c>
       <c r="P35" s="6" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="Q35" s="6" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17">
       <c r="A36" s="6">
         <v>49</v>
       </c>
@@ -2405,7 +2401,7 @@
         <v>42</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>43</v>
@@ -2418,7 +2414,7 @@
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6" t="s">
-        <v>69</v>
+        <v>145</v>
       </c>
       <c r="J36" s="6"/>
       <c r="K36" s="6"/>
@@ -2435,7 +2431,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17">
       <c r="A37" s="6">
         <v>51</v>
       </c>
@@ -2458,10 +2454,10 @@
         <v>1</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>69</v>
+        <v>141</v>
       </c>
       <c r="J37" s="6"/>
       <c r="K37" s="6"/>
@@ -2472,17 +2468,17 @@
       </c>
       <c r="N37" s="6"/>
       <c r="O37" s="6" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="P37" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="Q37" s="6" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17">
       <c r="A38" s="6">
         <v>51</v>
       </c>
@@ -2505,10 +2501,10 @@
         <v>1</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>69</v>
+        <v>142</v>
       </c>
       <c r="J38" s="6"/>
       <c r="K38" s="6"/>
@@ -2519,17 +2515,17 @@
       </c>
       <c r="N38" s="6"/>
       <c r="O38" s="6" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="P38" s="6" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="Q38" s="6" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17">
       <c r="A39" s="6">
         <v>51</v>
       </c>
@@ -2552,10 +2548,10 @@
         <v>1</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>69</v>
+        <v>143</v>
       </c>
       <c r="J39" s="6"/>
       <c r="K39" s="6"/>
@@ -2566,17 +2562,17 @@
       </c>
       <c r="N39" s="6"/>
       <c r="O39" s="6" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="P39" s="6" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="Q39" s="6" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17">
       <c r="A40" s="6">
         <v>55</v>
       </c>
@@ -2585,10 +2581,10 @@
         <v>47</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F40" s="9" t="s">
         <v>9</v>
@@ -2598,10 +2594,10 @@
       </c>
       <c r="H40" s="6"/>
       <c r="I40" s="6" t="s">
-        <v>69</v>
+        <v>144</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="K40" s="6">
         <v>30</v>
@@ -2616,13 +2612,13 @@
       <c r="P40" s="6"/>
       <c r="Q40" s="6"/>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17">
       <c r="A41" s="4">
         <v>56</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D41" s="11" t="s">
         <v>48</v>
@@ -2638,16 +2634,16 @@
       </c>
       <c r="H41" s="6"/>
       <c r="I41" s="6" t="s">
-        <v>61</v>
+        <v>145</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="K41" s="6">
         <v>1709</v>
       </c>
       <c r="L41" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M41" s="6">
         <f t="shared" si="0"/>
@@ -2660,13 +2656,13 @@
       <c r="P41" s="6"/>
       <c r="Q41" s="6"/>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17">
       <c r="A42" s="4">
         <v>56</v>
       </c>
       <c r="B42" s="4"/>
       <c r="C42" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D42" s="11" t="s">
         <v>48</v>
@@ -2678,10 +2674,10 @@
       <c r="G42" s="4"/>
       <c r="H42" s="6"/>
       <c r="I42" s="6" t="s">
-        <v>61</v>
+        <v>141</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="K42" s="6">
         <v>1699</v>

</xml_diff>

<commit_message>
Add mleader on ro
</commit_message>
<xml_diff>
--- a/cad/data.xlsx
+++ b/cad/data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\4 PProject\AutovaticCad\cad\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutomaticCad\cad\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09141FBE-A823-429A-BF2D-69024160C2EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5910" yWindow="0" windowWidth="19230" windowHeight="15750"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="3" r:id="rId1"/>
@@ -24,7 +25,7 @@
     <definedName name="d_ovik">#REF!</definedName>
     <definedName name="n_visio">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="184">
   <si>
     <t>Наименование</t>
   </si>
@@ -472,13 +473,127 @@
   </si>
   <si>
     <t>Зона 5</t>
+  </si>
+  <si>
+    <t>6.2</t>
+  </si>
+  <si>
+    <t>8.8</t>
+  </si>
+  <si>
+    <t>1.16</t>
+  </si>
+  <si>
+    <t>6.7</t>
+  </si>
+  <si>
+    <t>2.42</t>
+  </si>
+  <si>
+    <t>8.24</t>
+  </si>
+  <si>
+    <t>1.11</t>
+  </si>
+  <si>
+    <t>2.19</t>
+  </si>
+  <si>
+    <t>4.49</t>
+  </si>
+  <si>
+    <t>8.6</t>
+  </si>
+  <si>
+    <t>2.32</t>
+  </si>
+  <si>
+    <t>8.49</t>
+  </si>
+  <si>
+    <t>9.46</t>
+  </si>
+  <si>
+    <t>8.10</t>
+  </si>
+  <si>
+    <t>6.25</t>
+  </si>
+  <si>
+    <t>10.2</t>
+  </si>
+  <si>
+    <t>7.6</t>
+  </si>
+  <si>
+    <t>5.4</t>
+  </si>
+  <si>
+    <t>10.30</t>
+  </si>
+  <si>
+    <t>7.32</t>
+  </si>
+  <si>
+    <t>4.13</t>
+  </si>
+  <si>
+    <t>3.3</t>
+  </si>
+  <si>
+    <t>6.16</t>
+  </si>
+  <si>
+    <t>10.47</t>
+  </si>
+  <si>
+    <t>9.20</t>
+  </si>
+  <si>
+    <t>1.32</t>
+  </si>
+  <si>
+    <t>1.29</t>
+  </si>
+  <si>
+    <t>5.41</t>
+  </si>
+  <si>
+    <t>8.41</t>
+  </si>
+  <si>
+    <t>3.22</t>
+  </si>
+  <si>
+    <t>4.32</t>
+  </si>
+  <si>
+    <t>1.48</t>
+  </si>
+  <si>
+    <t>10.27</t>
+  </si>
+  <si>
+    <t>7.4</t>
+  </si>
+  <si>
+    <t>4.37</t>
+  </si>
+  <si>
+    <t>9.34</t>
+  </si>
+  <si>
+    <t>2.48</t>
+  </si>
+  <si>
+    <t>10.8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -556,7 +671,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -593,10 +708,17 @@
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Стиль 1" xfId="1"/>
+    <cellStyle name="Стиль 1" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -821,18 +943,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I36" sqref="I36"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R4" sqref="R4:R5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="7" style="15" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="15" customWidth="1"/>
     <col min="3" max="3" width="24.28515625" style="3" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="35.42578125" style="2" customWidth="1"/>
@@ -852,11 +974,11 @@
     <col min="19" max="16384" width="5.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="13" t="s">
         <v>115</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -905,11 +1027,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
-      <c r="A2" s="6">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6"/>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" s="14"/>
       <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
@@ -950,11 +1072,11 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:17">
-      <c r="A3" s="6">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6"/>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" s="14"/>
       <c r="C3" s="7" t="s">
         <v>7</v>
       </c>
@@ -991,11 +1113,11 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:17">
-      <c r="A4" s="6">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6"/>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" s="14"/>
       <c r="C4" s="7" t="s">
         <v>53</v>
       </c>
@@ -1032,11 +1154,11 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:17">
-      <c r="A5" s="6">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6"/>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5" s="14"/>
       <c r="C5" s="7" t="s">
         <v>12</v>
       </c>
@@ -1079,11 +1201,11 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:17">
-      <c r="A6" s="6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="B6" s="14">
         <v>1</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -1130,11 +1252,11 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:17">
-      <c r="A7" s="6">
-        <v>5</v>
-      </c>
-      <c r="B7" s="6">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7" s="14">
         <v>2</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -1181,11 +1303,11 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:17">
-      <c r="A8" s="6">
-        <v>6</v>
-      </c>
-      <c r="B8" s="6">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8" s="14">
         <v>1</v>
       </c>
       <c r="C8" s="7" t="s">
@@ -1224,11 +1346,11 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:17">
-      <c r="A9" s="6">
-        <v>6</v>
-      </c>
-      <c r="B9" s="6">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="B9" s="14">
         <v>2</v>
       </c>
       <c r="C9" s="7" t="s">
@@ -1267,11 +1389,11 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:17">
-      <c r="A10" s="6">
-        <v>12</v>
-      </c>
-      <c r="B10" s="6"/>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="B10" s="14"/>
       <c r="C10" s="7" t="s">
         <v>23</v>
       </c>
@@ -1312,11 +1434,11 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:17">
-      <c r="A11" s="6">
-        <v>12.1</v>
-      </c>
-      <c r="B11" s="6"/>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="B11" s="14"/>
       <c r="C11" s="7" t="s">
         <v>26</v>
       </c>
@@ -1351,11 +1473,11 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:17">
-      <c r="A12" s="6">
-        <v>13</v>
-      </c>
-      <c r="B12" s="6"/>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="B12" s="14"/>
       <c r="C12" s="7" t="s">
         <v>54</v>
       </c>
@@ -1392,11 +1514,11 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:17">
-      <c r="A13" s="6">
-        <v>14</v>
-      </c>
-      <c r="B13" s="6"/>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="B13" s="14"/>
       <c r="C13" s="7" t="s">
         <v>12</v>
       </c>
@@ -1439,11 +1561,11 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:17">
-      <c r="A14" s="6">
-        <v>15</v>
-      </c>
-      <c r="B14" s="6"/>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="B14" s="14"/>
       <c r="C14" s="7" t="s">
         <v>28</v>
       </c>
@@ -1480,11 +1602,11 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:17">
-      <c r="A15" s="6">
-        <v>17</v>
-      </c>
-      <c r="B15" s="6"/>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="B15" s="14"/>
       <c r="C15" s="7" t="s">
         <v>23</v>
       </c>
@@ -1525,11 +1647,11 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="13.5" customHeight="1">
-      <c r="A16" s="6">
-        <v>17.100000000000001</v>
-      </c>
-      <c r="B16" s="6"/>
+    <row r="16" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="B16" s="14"/>
       <c r="C16" s="7" t="s">
         <v>26</v>
       </c>
@@ -1566,11 +1688,11 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:17">
-      <c r="A17" s="6">
-        <v>18</v>
-      </c>
-      <c r="B17" s="6"/>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="B17" s="14"/>
       <c r="C17" s="7" t="s">
         <v>54</v>
       </c>
@@ -1607,11 +1729,11 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:17">
-      <c r="A18" s="6">
-        <v>19</v>
-      </c>
-      <c r="B18" s="6"/>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="B18" s="14"/>
       <c r="C18" s="7" t="s">
         <v>12</v>
       </c>
@@ -1654,11 +1776,11 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:17">
-      <c r="A19" s="6">
-        <v>20</v>
-      </c>
-      <c r="B19" s="6"/>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="B19" s="14"/>
       <c r="C19" s="7" t="s">
         <v>3</v>
       </c>
@@ -1693,11 +1815,11 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:17">
-      <c r="A20" s="6">
-        <v>21</v>
-      </c>
-      <c r="B20" s="6"/>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="B20" s="14"/>
       <c r="C20" s="7" t="s">
         <v>15</v>
       </c>
@@ -1742,11 +1864,11 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:17">
-      <c r="A21" s="6">
-        <v>22</v>
-      </c>
-      <c r="B21" s="6"/>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="B21" s="14"/>
       <c r="C21" s="7" t="s">
         <v>34</v>
       </c>
@@ -1773,11 +1895,11 @@
       <c r="P21" s="6"/>
       <c r="Q21" s="6"/>
     </row>
-    <row r="22" spans="1:17">
-      <c r="A22" s="6">
-        <v>23</v>
-      </c>
-      <c r="B22" s="6"/>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="B22" s="14"/>
       <c r="C22" s="7" t="s">
         <v>18</v>
       </c>
@@ -1814,11 +1936,11 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:17">
-      <c r="A23" s="6">
-        <v>29</v>
-      </c>
-      <c r="B23" s="6"/>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="B23" s="14"/>
       <c r="C23" s="10" t="s">
         <v>28</v>
       </c>
@@ -1863,11 +1985,11 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:17">
-      <c r="A24" s="6">
-        <v>30</v>
-      </c>
-      <c r="B24" s="6">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="B24" s="14">
         <v>1</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -1914,11 +2036,11 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:17">
-      <c r="A25" s="6">
-        <v>30</v>
-      </c>
-      <c r="B25" s="6">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="B25" s="14">
         <v>2</v>
       </c>
       <c r="C25" s="7" t="s">
@@ -1965,11 +2087,11 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:17">
-      <c r="A26" s="6">
-        <v>31</v>
-      </c>
-      <c r="B26" s="6">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="B26" s="14">
         <v>1</v>
       </c>
       <c r="C26" s="7" t="s">
@@ -2002,11 +2124,11 @@
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
     </row>
-    <row r="27" spans="1:17">
-      <c r="A27" s="6">
-        <v>31</v>
-      </c>
-      <c r="B27" s="6">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="B27" s="14">
         <v>2</v>
       </c>
       <c r="C27" s="7" t="s">
@@ -2039,11 +2161,11 @@
       <c r="P27" s="6"/>
       <c r="Q27" s="6"/>
     </row>
-    <row r="28" spans="1:17">
-      <c r="A28" s="6">
-        <v>32</v>
-      </c>
-      <c r="B28" s="6">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="B28" s="14">
         <v>1</v>
       </c>
       <c r="C28" s="7" t="s">
@@ -2082,11 +2204,11 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:17">
-      <c r="A29" s="6">
-        <v>32</v>
-      </c>
-      <c r="B29" s="6">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="B29" s="14">
         <v>2</v>
       </c>
       <c r="C29" s="7" t="s">
@@ -2125,11 +2247,11 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:17">
-      <c r="A30" s="6">
-        <v>34</v>
-      </c>
-      <c r="B30" s="6"/>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="B30" s="14"/>
       <c r="C30" s="7" t="s">
         <v>21</v>
       </c>
@@ -2167,11 +2289,11 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:17">
-      <c r="A31" s="6">
-        <v>39</v>
-      </c>
-      <c r="B31" s="6">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="B31" s="14">
         <v>1</v>
       </c>
       <c r="C31" s="7" t="s">
@@ -2212,11 +2334,11 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:17">
-      <c r="A32" s="6">
-        <v>39</v>
-      </c>
-      <c r="B32" s="6">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="B32" s="14">
         <v>2</v>
       </c>
       <c r="C32" s="7" t="s">
@@ -2257,11 +2379,11 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:17">
-      <c r="A33" s="6">
-        <v>39</v>
-      </c>
-      <c r="B33" s="6">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="B33" s="14">
         <v>3</v>
       </c>
       <c r="C33" s="7" t="s">
@@ -2302,11 +2424,11 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:17">
-      <c r="A34" s="6">
-        <v>39</v>
-      </c>
-      <c r="B34" s="6">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="B34" s="14">
         <v>4</v>
       </c>
       <c r="C34" s="7" t="s">
@@ -2347,11 +2469,11 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:17">
-      <c r="A35" s="6">
-        <v>48</v>
-      </c>
-      <c r="B35" s="6"/>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="B35" s="14"/>
       <c r="C35" s="7" t="s">
         <v>40</v>
       </c>
@@ -2392,11 +2514,11 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:17">
-      <c r="A36" s="6">
-        <v>49</v>
-      </c>
-      <c r="B36" s="6"/>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="B36" s="14"/>
       <c r="C36" s="7" t="s">
         <v>42</v>
       </c>
@@ -2431,11 +2553,11 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:17">
-      <c r="A37" s="6">
-        <v>51</v>
-      </c>
-      <c r="B37" s="6">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="B37" s="14">
         <v>1</v>
       </c>
       <c r="C37" s="7" t="s">
@@ -2478,11 +2600,11 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:17">
-      <c r="A38" s="6">
-        <v>51</v>
-      </c>
-      <c r="B38" s="6">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="B38" s="14">
         <v>2</v>
       </c>
       <c r="C38" s="7" t="s">
@@ -2525,11 +2647,11 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:17">
-      <c r="A39" s="6">
-        <v>51</v>
-      </c>
-      <c r="B39" s="6">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="B39" s="14">
         <v>3</v>
       </c>
       <c r="C39" s="7" t="s">
@@ -2572,11 +2694,11 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:17">
-      <c r="A40" s="6">
-        <v>55</v>
-      </c>
-      <c r="B40" s="6"/>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="B40" s="14"/>
       <c r="C40" s="7" t="s">
         <v>47</v>
       </c>
@@ -2612,11 +2734,11 @@
       <c r="P40" s="6"/>
       <c r="Q40" s="6"/>
     </row>
-    <row r="41" spans="1:17">
-      <c r="A41" s="4">
-        <v>56</v>
-      </c>
-      <c r="B41" s="4"/>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="B41" s="13"/>
       <c r="C41" s="5" t="s">
         <v>66</v>
       </c>
@@ -2656,11 +2778,11 @@
       <c r="P41" s="6"/>
       <c r="Q41" s="6"/>
     </row>
-    <row r="42" spans="1:17">
-      <c r="A42" s="4">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A42" s="13">
         <v>56</v>
       </c>
-      <c r="B42" s="4"/>
+      <c r="B42" s="13"/>
       <c r="C42" s="5" t="s">
         <v>66</v>
       </c>

</xml_diff>